<commit_message>
오전 01:05 2021-01-09 npm project initialize
</commit_message>
<xml_diff>
--- a/Communication/일정표(매일수정).xlsx
+++ b/Communication/일정표(매일수정).xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.5454"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="7710"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="28545" windowHeight="11880"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="26">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="27">
   <x:si>
     <x:t>9주차</x:t>
   </x:si>
   <x:si>
     <x:t>CSS 폼 디자인, UI 설계 및 시각적 기능 구현</x:t>
+  </x:si>
+  <x:si>
+    <x:t>환경구축 세팅
+및 협의 
+HLS 알아보기
+MongoDB알아보기</x:t>
   </x:si>
   <x:si>
     <x:t>o</x:t>
@@ -62,9 +68,6 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">부기능, 추가 희망기능 등등 추가하는 주 .() </x:t>
-  </x:si>
-  <x:si>
-    <x:t>8주차</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Start : 
@@ -73,9 +76,14 @@
 (DBMS) MongoDB,
 (Cloud) AWS 
 Discord 시간 : 18:00 ~ 23:00 (평일) /  주말은 자습
+MongoDB aws 연결하는법
+aws lambda 알아보기 
 *업무분담은 프로젝트 진행중에 나누도록 하고
 * 웹 에서 어떻게 영상이 개시되고 실시간 중계하고 , 저장되고, 송출하고, 등등 어떻게 하는지 , 무슨 원리로 하는지 해당 제공 함수가 있는지, 프레임워크가 있는지 알아보기
 </x:t>
+  </x:si>
+  <x:si>
+    <x:t>8주차</x:t>
   </x:si>
   <x:si>
     <x:t>3주차</x:t>
@@ -530,7 +538,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="38">
+  <x:cellXfs count="39">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -842,6 +850,19 @@
     <x:xf numFmtId="0" fontId="8" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="general" vertical="center" wrapText="1"/>
     </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
@@ -1610,7 +1631,7 @@
   <x:dimension ref="A1:M44"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="K3" activeCellId="0" sqref="K3:K3"/>
+      <x:selection activeCell="M2" activeCellId="0" sqref="M2:M3"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
@@ -1627,7 +1648,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:12" s="3" customFormat="1" ht="84" customHeight="1">
       <x:c r="A1" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B1" s="13">
         <x:v>44200</x:v>
@@ -1652,72 +1673,72 @@
       </x:c>
       <x:c r="I1" s="14"/>
       <x:c r="J1" s="13" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="K1" s="13" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="L1" s="15" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="K1" s="13" t="s">
+    </x:row>
+    <x:row r="2" spans="1:13" s="4" customFormat="1" ht="162" customHeight="1">
+      <x:c r="A2" s="16" t="s">
         <x:v>5</x:v>
-      </x:c>
-      <x:c r="L1" s="15" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:13" s="4" customFormat="1" ht="84" customHeight="1">
-      <x:c r="A2" s="16" t="s">
-        <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="27"/>
       <x:c r="C2" s="27"/>
       <x:c r="D2" s="27"/>
       <x:c r="E2" s="31" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F2" s="32" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="G2" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G2" s="37" t="s">
+        <x:v>2</x:v>
       </x:c>
       <x:c r="H2" s="32" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="I2" s="7"/>
       <x:c r="J2" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K2" s="32" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="L2" s="37" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="L2" s="38" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="M2" s="25"/>
     </x:row>
-    <x:row r="3" spans="1:13" s="3" customFormat="1" ht="84" customHeight="1">
+    <x:row r="3" spans="1:13" s="3" customFormat="1" ht="162" customHeight="1">
       <x:c r="A3" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B3" s="28"/>
       <x:c r="C3" s="29"/>
       <x:c r="D3" s="29"/>
       <x:c r="E3" s="9" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="F3" s="9" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G3" s="9"/>
       <x:c r="H3" s="9"/>
       <x:c r="I3" s="5"/>
       <x:c r="J3" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="K3" s="8"/>
       <x:c r="L3" s="23"/>
       <x:c r="M3" s="26"/>
     </x:row>
-    <x:row r="4" spans="1:12" s="4" customFormat="1" ht="84" customHeight="1">
+    <x:row r="4" spans="1:12" s="4" customFormat="1" ht="162" customHeight="1">
       <x:c r="A4" s="18" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B4" s="30"/>
       <x:c r="C4" s="30"/>
@@ -1728,7 +1749,7 @@
       <x:c r="H4" s="19"/>
       <x:c r="I4" s="20"/>
       <x:c r="J4" s="21" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K4" s="21"/>
       <x:c r="L4" s="24"/>
@@ -1736,7 +1757,7 @@
     <x:row r="5" ht="23.25" customHeight="1"/>
     <x:row r="6" spans="1:12" ht="91.5" customHeight="1">
       <x:c r="A6" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B6" s="13">
         <x:v>44207</x:v>
@@ -1761,18 +1782,18 @@
       </x:c>
       <x:c r="I6" s="14"/>
       <x:c r="J6" s="13" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="K6" s="13" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="L6" s="15" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="K6" s="13" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="L6" s="15" t="s">
-        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:12" ht="91.5" customHeight="1">
       <x:c r="A7" s="16" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B7" s="6"/>
       <x:c r="C7" s="6"/>
@@ -1783,16 +1804,16 @@
       <x:c r="H7" s="6"/>
       <x:c r="I7" s="7"/>
       <x:c r="J7" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K7" s="32" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L7" s="22"/>
     </x:row>
     <x:row r="8" spans="1:12" ht="91.5" customHeight="1">
       <x:c r="A8" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B8" s="9"/>
       <x:c r="C8" s="10"/>
@@ -1803,14 +1824,14 @@
       <x:c r="H8" s="9"/>
       <x:c r="I8" s="5"/>
       <x:c r="J8" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="K8" s="8"/>
       <x:c r="L8" s="23"/>
     </x:row>
     <x:row r="9" spans="1:12" ht="91.5" customHeight="1">
       <x:c r="A9" s="18" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B9" s="19"/>
       <x:c r="C9" s="19"/>
@@ -1821,14 +1842,14 @@
       <x:c r="H9" s="19"/>
       <x:c r="I9" s="20"/>
       <x:c r="J9" s="21" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K9" s="21"/>
       <x:c r="L9" s="24"/>
     </x:row>
     <x:row r="11" spans="1:12" ht="80.25" customHeight="1">
       <x:c r="A11" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B11" s="13">
         <x:v>44214</x:v>
@@ -1853,18 +1874,18 @@
       </x:c>
       <x:c r="I11" s="14"/>
       <x:c r="J11" s="13" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="K11" s="13" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="L11" s="15" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="K11" s="13" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="L11" s="15" t="s">
-        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:12" ht="80.25" customHeight="1">
       <x:c r="A12" s="16" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B12" s="6"/>
       <x:c r="C12" s="6"/>
@@ -1875,16 +1896,16 @@
       <x:c r="H12" s="6"/>
       <x:c r="I12" s="7"/>
       <x:c r="J12" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K12" s="6" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L12" s="22"/>
     </x:row>
     <x:row r="13" spans="1:12" ht="80.25" customHeight="1">
       <x:c r="A13" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B13" s="9"/>
       <x:c r="C13" s="10"/>
@@ -1895,14 +1916,14 @@
       <x:c r="H13" s="9"/>
       <x:c r="I13" s="5"/>
       <x:c r="J13" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="K13" s="8"/>
       <x:c r="L13" s="23"/>
     </x:row>
     <x:row r="14" spans="1:12" ht="80.25" customHeight="1">
       <x:c r="A14" s="18" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B14" s="19"/>
       <x:c r="C14" s="19"/>
@@ -1913,14 +1934,14 @@
       <x:c r="H14" s="19"/>
       <x:c r="I14" s="20"/>
       <x:c r="J14" s="21" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K14" s="21"/>
       <x:c r="L14" s="24"/>
     </x:row>
     <x:row r="16" spans="1:12" ht="81" customHeight="1">
       <x:c r="A16" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B16" s="13">
         <x:v>44221</x:v>
@@ -1945,18 +1966,18 @@
       </x:c>
       <x:c r="I16" s="14"/>
       <x:c r="J16" s="13" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="K16" s="13" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="L16" s="15" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="K16" s="13" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="L16" s="15" t="s">
-        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:12" ht="81" customHeight="1">
       <x:c r="A17" s="16" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B17" s="6"/>
       <x:c r="C17" s="6"/>
@@ -1967,16 +1988,16 @@
       <x:c r="H17" s="6"/>
       <x:c r="I17" s="7"/>
       <x:c r="J17" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K17" s="32" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L17" s="22"/>
     </x:row>
     <x:row r="18" spans="1:12" ht="81" customHeight="1">
       <x:c r="A18" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B18" s="9"/>
       <x:c r="C18" s="10"/>
@@ -1987,14 +2008,14 @@
       <x:c r="H18" s="9"/>
       <x:c r="I18" s="5"/>
       <x:c r="J18" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="K18" s="8"/>
       <x:c r="L18" s="23"/>
     </x:row>
     <x:row r="19" spans="1:12" ht="81" customHeight="1">
       <x:c r="A19" s="18" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B19" s="19"/>
       <x:c r="C19" s="19"/>
@@ -2005,14 +2026,14 @@
       <x:c r="H19" s="19"/>
       <x:c r="I19" s="20"/>
       <x:c r="J19" s="21" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K19" s="21"/>
       <x:c r="L19" s="24"/>
     </x:row>
     <x:row r="21" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A21" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B21" s="13">
         <x:v>44228</x:v>
@@ -2037,18 +2058,18 @@
       </x:c>
       <x:c r="I21" s="14"/>
       <x:c r="J21" s="13" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="K21" s="13" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="L21" s="15" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="K21" s="13" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="L21" s="15" t="s">
-        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A22" s="16" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B22" s="6"/>
       <x:c r="C22" s="6"/>
@@ -2059,7 +2080,7 @@
       <x:c r="H22" s="6"/>
       <x:c r="I22" s="7"/>
       <x:c r="J22" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K22" s="6" t="s">
         <x:v>1</x:v>
@@ -2068,7 +2089,7 @@
     </x:row>
     <x:row r="23" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A23" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B23" s="9"/>
       <x:c r="C23" s="10"/>
@@ -2079,14 +2100,14 @@
       <x:c r="H23" s="9"/>
       <x:c r="I23" s="5"/>
       <x:c r="J23" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="K23" s="8"/>
       <x:c r="L23" s="23"/>
     </x:row>
     <x:row r="24" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A24" s="18" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B24" s="19"/>
       <x:c r="C24" s="19"/>
@@ -2097,14 +2118,14 @@
       <x:c r="H24" s="19"/>
       <x:c r="I24" s="20"/>
       <x:c r="J24" s="21" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K24" s="21"/>
       <x:c r="L24" s="24"/>
     </x:row>
     <x:row r="26" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A26" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B26" s="13">
         <x:v>44235</x:v>
@@ -2129,18 +2150,18 @@
       </x:c>
       <x:c r="I26" s="14"/>
       <x:c r="J26" s="13" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="K26" s="13" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="L26" s="15" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="K26" s="13" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="L26" s="15" t="s">
-        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A27" s="16" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B27" s="6"/>
       <x:c r="C27" s="6"/>
@@ -2151,7 +2172,7 @@
       <x:c r="H27" s="6"/>
       <x:c r="I27" s="7"/>
       <x:c r="J27" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K27" s="6" t="s">
         <x:v>1</x:v>
@@ -2160,7 +2181,7 @@
     </x:row>
     <x:row r="28" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A28" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B28" s="9"/>
       <x:c r="C28" s="10"/>
@@ -2171,14 +2192,14 @@
       <x:c r="H28" s="9"/>
       <x:c r="I28" s="5"/>
       <x:c r="J28" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="K28" s="8"/>
       <x:c r="L28" s="23"/>
     </x:row>
     <x:row r="29" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A29" s="18" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B29" s="19"/>
       <x:c r="C29" s="19"/>
@@ -2189,14 +2210,14 @@
       <x:c r="H29" s="19"/>
       <x:c r="I29" s="20"/>
       <x:c r="J29" s="21" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K29" s="21"/>
       <x:c r="L29" s="24"/>
     </x:row>
     <x:row r="31" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A31" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B31" s="13">
         <x:v>44242</x:v>
@@ -2221,18 +2242,18 @@
       </x:c>
       <x:c r="I31" s="14"/>
       <x:c r="J31" s="13" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="K31" s="13" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L31" s="15" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="K31" s="13" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="L31" s="15" t="s">
-        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A32" s="16" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B32" s="6"/>
       <x:c r="C32" s="6"/>
@@ -2243,16 +2264,16 @@
       <x:c r="H32" s="6"/>
       <x:c r="I32" s="7"/>
       <x:c r="J32" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K32" s="6" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="L32" s="22"/>
     </x:row>
     <x:row r="33" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A33" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B33" s="9"/>
       <x:c r="C33" s="10"/>
@@ -2263,14 +2284,14 @@
       <x:c r="H33" s="9"/>
       <x:c r="I33" s="5"/>
       <x:c r="J33" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="K33" s="8"/>
       <x:c r="L33" s="23"/>
     </x:row>
     <x:row r="34" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A34" s="18" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B34" s="19"/>
       <x:c r="C34" s="19"/>
@@ -2281,14 +2302,14 @@
       <x:c r="H34" s="19"/>
       <x:c r="I34" s="20"/>
       <x:c r="J34" s="21" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K34" s="21"/>
       <x:c r="L34" s="24"/>
     </x:row>
     <x:row r="36" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A36" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B36" s="13">
         <x:v>44249</x:v>
@@ -2313,18 +2334,18 @@
       </x:c>
       <x:c r="I36" s="14"/>
       <x:c r="J36" s="13" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="K36" s="13" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="L36" s="15" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="K36" s="13" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="L36" s="15" t="s">
-        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A37" s="16" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B37" s="6"/>
       <x:c r="C37" s="6"/>
@@ -2335,14 +2356,14 @@
       <x:c r="H37" s="6"/>
       <x:c r="I37" s="7"/>
       <x:c r="J37" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K37" s="6"/>
       <x:c r="L37" s="22"/>
     </x:row>
     <x:row r="38" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A38" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B38" s="9"/>
       <x:c r="C38" s="10"/>
@@ -2353,14 +2374,14 @@
       <x:c r="H38" s="9"/>
       <x:c r="I38" s="5"/>
       <x:c r="J38" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="K38" s="8"/>
       <x:c r="L38" s="23"/>
     </x:row>
     <x:row r="39" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A39" s="18" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B39" s="19"/>
       <x:c r="C39" s="19"/>
@@ -2371,14 +2392,14 @@
       <x:c r="H39" s="19"/>
       <x:c r="I39" s="20"/>
       <x:c r="J39" s="21" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K39" s="21"/>
       <x:c r="L39" s="24"/>
     </x:row>
     <x:row r="41" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A41" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B41" s="13">
         <x:v>44256</x:v>
@@ -2403,18 +2424,18 @@
       </x:c>
       <x:c r="I41" s="14"/>
       <x:c r="J41" s="13" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="K41" s="13" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="L41" s="15" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A42" s="16" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B42" s="6"/>
       <x:c r="C42" s="6"/>
@@ -2423,18 +2444,18 @@
       <x:c r="F42" s="6"/>
       <x:c r="G42" s="6"/>
       <x:c r="H42" s="34" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="I42" s="7"/>
       <x:c r="J42" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K42" s="6"/>
       <x:c r="L42" s="22"/>
     </x:row>
     <x:row r="43" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A43" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B43" s="9"/>
       <x:c r="C43" s="10"/>
@@ -2445,14 +2466,14 @@
       <x:c r="H43" s="35"/>
       <x:c r="I43" s="5"/>
       <x:c r="J43" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="K43" s="8"/>
       <x:c r="L43" s="23"/>
     </x:row>
     <x:row r="44" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A44" s="18" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B44" s="19"/>
       <x:c r="C44" s="19"/>
@@ -2463,7 +2484,7 @@
       <x:c r="H44" s="36"/>
       <x:c r="I44" s="20"/>
       <x:c r="J44" s="21" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K44" s="21"/>
       <x:c r="L44" s="24"/>

</xml_diff>

<commit_message>
20210112 15:23 일정표 수정
</commit_message>
<xml_diff>
--- a/Communication/일정표(매일수정).xlsx
+++ b/Communication/일정표(매일수정).xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.5454"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="28545" windowHeight="11880"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="7710"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="27">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="30">
   <x:si>
     <x:t>9주차</x:t>
   </x:si>
@@ -38,6 +38,9 @@
   </x:si>
   <x:si>
     <x:t>1주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">지난 주말 환경셋팅을 다못하는 바람에 시간이 약간 새었음 </x:t>
   </x:si>
   <x:si>
     <x:t>문제점, 해결법</x:t>
@@ -83,7 +86,14 @@
 </x:t>
   </x:si>
   <x:si>
+    <x:t>Boiler-Plate 제작</x:t>
+  </x:si>
+  <x:si>
     <x:t>8주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>아무래도 밤늦게 진행하다 보니 졸리기도 하고 효율이 좋지 않은것 같다. 
+일찍하는게 좋지않나 싶다</x:t>
   </x:si>
   <x:si>
     <x:t>3주차</x:t>
@@ -1630,8 +1640,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="A1:M44"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="M2" activeCellId="0" sqref="M2:M3"/>
+    <x:sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="D8" activeCellId="0" sqref="D8:D8"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
@@ -1646,7 +1656,7 @@
     <x:col min="14" max="16384" width="9" style="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:12" s="3" customFormat="1" ht="84" customHeight="1">
+    <x:row r="1" spans="1:12" s="3" customFormat="1" ht="114" customHeight="1">
       <x:c r="A1" s="12" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -1673,16 +1683,16 @@
       </x:c>
       <x:c r="I1" s="14"/>
       <x:c r="J1" s="13" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="K1" s="13" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="L1" s="15" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:13" s="4" customFormat="1" ht="162" customHeight="1">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:13" s="4" customFormat="1" ht="114" customHeight="1">
       <x:c r="A2" s="16" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -1690,32 +1700,32 @@
       <x:c r="C2" s="27"/>
       <x:c r="D2" s="27"/>
       <x:c r="E2" s="31" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F2" s="32" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G2" s="37" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="H2" s="32" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="I2" s="7"/>
       <x:c r="J2" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
       <x:c r="K2" s="32" t="s">
-        <x:v>23</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="L2" s="38" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="M2" s="25"/>
     </x:row>
-    <x:row r="3" spans="1:13" s="3" customFormat="1" ht="162" customHeight="1">
+    <x:row r="3" spans="1:13" s="3" customFormat="1" ht="114" customHeight="1">
       <x:c r="A3" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B3" s="28"/>
       <x:c r="C3" s="29"/>
@@ -1724,21 +1734,21 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="F3" s="9" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="G3" s="9"/>
       <x:c r="H3" s="9"/>
       <x:c r="I3" s="5"/>
       <x:c r="J3" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="K3" s="8"/>
       <x:c r="L3" s="23"/>
       <x:c r="M3" s="26"/>
     </x:row>
-    <x:row r="4" spans="1:12" s="4" customFormat="1" ht="162" customHeight="1">
+    <x:row r="4" spans="1:12" s="4" customFormat="1" ht="114" customHeight="1">
       <x:c r="A4" s="18" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B4" s="30"/>
       <x:c r="C4" s="30"/>
@@ -1749,7 +1759,7 @@
       <x:c r="H4" s="19"/>
       <x:c r="I4" s="20"/>
       <x:c r="J4" s="21" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="K4" s="21"/>
       <x:c r="L4" s="24"/>
@@ -1782,22 +1792,28 @@
       </x:c>
       <x:c r="I6" s="14"/>
       <x:c r="J6" s="13" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="K6" s="13" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L6" s="15" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="K6" s="13" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="L6" s="15" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:12" ht="91.5" customHeight="1">
       <x:c r="A7" s="16" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B7" s="6"/>
-      <x:c r="C7" s="6"/>
-      <x:c r="D7" s="6"/>
+      <x:c r="B7" s="6" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C7" s="6" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D7" s="6" t="s">
+        <x:v>18</x:v>
+      </x:c>
       <x:c r="E7" s="6"/>
       <x:c r="F7" s="6"/>
       <x:c r="G7" s="6"/>
@@ -1807,15 +1823,17 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="K7" s="32" t="s">
-        <x:v>25</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="L7" s="22"/>
     </x:row>
     <x:row r="8" spans="1:12" ht="91.5" customHeight="1">
       <x:c r="A8" s="17" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B8" s="9"/>
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B8" s="9" t="s">
+        <x:v>7</x:v>
+      </x:c>
       <x:c r="C8" s="10"/>
       <x:c r="D8" s="10"/>
       <x:c r="E8" s="11"/>
@@ -1824,16 +1842,18 @@
       <x:c r="H8" s="9"/>
       <x:c r="I8" s="5"/>
       <x:c r="J8" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="K8" s="8"/>
       <x:c r="L8" s="23"/>
     </x:row>
     <x:row r="9" spans="1:12" ht="91.5" customHeight="1">
       <x:c r="A9" s="18" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B9" s="19"/>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B9" s="19" t="s">
+        <x:v>20</x:v>
+      </x:c>
       <x:c r="C9" s="19"/>
       <x:c r="D9" s="19"/>
       <x:c r="E9" s="19"/>
@@ -1842,7 +1862,7 @@
       <x:c r="H9" s="19"/>
       <x:c r="I9" s="20"/>
       <x:c r="J9" s="21" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="K9" s="21"/>
       <x:c r="L9" s="24"/>
@@ -1874,13 +1894,13 @@
       </x:c>
       <x:c r="I11" s="14"/>
       <x:c r="J11" s="13" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="K11" s="13" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L11" s="15" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="K11" s="13" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="L11" s="15" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:12" ht="80.25" customHeight="1">
@@ -1899,13 +1919,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="K12" s="6" t="s">
-        <x:v>25</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="L12" s="22"/>
     </x:row>
     <x:row r="13" spans="1:12" ht="80.25" customHeight="1">
       <x:c r="A13" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="9"/>
       <x:c r="C13" s="10"/>
@@ -1916,14 +1936,14 @@
       <x:c r="H13" s="9"/>
       <x:c r="I13" s="5"/>
       <x:c r="J13" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="K13" s="8"/>
       <x:c r="L13" s="23"/>
     </x:row>
     <x:row r="14" spans="1:12" ht="80.25" customHeight="1">
       <x:c r="A14" s="18" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B14" s="19"/>
       <x:c r="C14" s="19"/>
@@ -1934,7 +1954,7 @@
       <x:c r="H14" s="19"/>
       <x:c r="I14" s="20"/>
       <x:c r="J14" s="21" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="K14" s="21"/>
       <x:c r="L14" s="24"/>
@@ -1966,13 +1986,13 @@
       </x:c>
       <x:c r="I16" s="14"/>
       <x:c r="J16" s="13" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="K16" s="13" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="L16" s="15" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="K16" s="13" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="L16" s="15" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:12" ht="81" customHeight="1">
@@ -1991,13 +2011,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="K17" s="32" t="s">
-        <x:v>25</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="L17" s="22"/>
     </x:row>
     <x:row r="18" spans="1:12" ht="81" customHeight="1">
       <x:c r="A18" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B18" s="9"/>
       <x:c r="C18" s="10"/>
@@ -2008,14 +2028,14 @@
       <x:c r="H18" s="9"/>
       <x:c r="I18" s="5"/>
       <x:c r="J18" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="K18" s="8"/>
       <x:c r="L18" s="23"/>
     </x:row>
     <x:row r="19" spans="1:12" ht="81" customHeight="1">
       <x:c r="A19" s="18" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B19" s="19"/>
       <x:c r="C19" s="19"/>
@@ -2026,7 +2046,7 @@
       <x:c r="H19" s="19"/>
       <x:c r="I19" s="20"/>
       <x:c r="J19" s="21" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="K19" s="21"/>
       <x:c r="L19" s="24"/>
@@ -2058,13 +2078,13 @@
       </x:c>
       <x:c r="I21" s="14"/>
       <x:c r="J21" s="13" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="K21" s="13" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="L21" s="15" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="K21" s="13" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="L21" s="15" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:12" ht="106.5" customHeight="1">
@@ -2089,7 +2109,7 @@
     </x:row>
     <x:row r="23" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A23" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B23" s="9"/>
       <x:c r="C23" s="10"/>
@@ -2100,14 +2120,14 @@
       <x:c r="H23" s="9"/>
       <x:c r="I23" s="5"/>
       <x:c r="J23" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="K23" s="8"/>
       <x:c r="L23" s="23"/>
     </x:row>
     <x:row r="24" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A24" s="18" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B24" s="19"/>
       <x:c r="C24" s="19"/>
@@ -2118,7 +2138,7 @@
       <x:c r="H24" s="19"/>
       <x:c r="I24" s="20"/>
       <x:c r="J24" s="21" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="K24" s="21"/>
       <x:c r="L24" s="24"/>
@@ -2150,13 +2170,13 @@
       </x:c>
       <x:c r="I26" s="14"/>
       <x:c r="J26" s="13" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="K26" s="13" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="L26" s="15" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="K26" s="13" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="L26" s="15" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:12" ht="97.5" customHeight="1">
@@ -2181,7 +2201,7 @@
     </x:row>
     <x:row r="28" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A28" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B28" s="9"/>
       <x:c r="C28" s="10"/>
@@ -2192,14 +2212,14 @@
       <x:c r="H28" s="9"/>
       <x:c r="I28" s="5"/>
       <x:c r="J28" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="K28" s="8"/>
       <x:c r="L28" s="23"/>
     </x:row>
     <x:row r="29" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A29" s="18" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B29" s="19"/>
       <x:c r="C29" s="19"/>
@@ -2210,7 +2230,7 @@
       <x:c r="H29" s="19"/>
       <x:c r="I29" s="20"/>
       <x:c r="J29" s="21" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="K29" s="21"/>
       <x:c r="L29" s="24"/>
@@ -2242,13 +2262,13 @@
       </x:c>
       <x:c r="I31" s="14"/>
       <x:c r="J31" s="13" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="K31" s="13" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="L31" s="15" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="K31" s="13" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="L31" s="15" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:12" ht="108.75" customHeight="1">
@@ -2267,13 +2287,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="K32" s="6" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="L32" s="22"/>
     </x:row>
     <x:row r="33" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A33" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B33" s="9"/>
       <x:c r="C33" s="10"/>
@@ -2284,14 +2304,14 @@
       <x:c r="H33" s="9"/>
       <x:c r="I33" s="5"/>
       <x:c r="J33" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="K33" s="8"/>
       <x:c r="L33" s="23"/>
     </x:row>
     <x:row r="34" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A34" s="18" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B34" s="19"/>
       <x:c r="C34" s="19"/>
@@ -2302,7 +2322,7 @@
       <x:c r="H34" s="19"/>
       <x:c r="I34" s="20"/>
       <x:c r="J34" s="21" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="K34" s="21"/>
       <x:c r="L34" s="24"/>
@@ -2334,13 +2354,13 @@
       </x:c>
       <x:c r="I36" s="14"/>
       <x:c r="J36" s="13" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="K36" s="13" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="L36" s="15" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="K36" s="13" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="L36" s="15" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:12" ht="109.5" customHeight="1">
@@ -2363,7 +2383,7 @@
     </x:row>
     <x:row r="38" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A38" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B38" s="9"/>
       <x:c r="C38" s="10"/>
@@ -2374,14 +2394,14 @@
       <x:c r="H38" s="9"/>
       <x:c r="I38" s="5"/>
       <x:c r="J38" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="K38" s="8"/>
       <x:c r="L38" s="23"/>
     </x:row>
     <x:row r="39" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A39" s="18" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B39" s="19"/>
       <x:c r="C39" s="19"/>
@@ -2392,7 +2412,7 @@
       <x:c r="H39" s="19"/>
       <x:c r="I39" s="20"/>
       <x:c r="J39" s="21" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="K39" s="21"/>
       <x:c r="L39" s="24"/>
@@ -2424,13 +2444,13 @@
       </x:c>
       <x:c r="I41" s="14"/>
       <x:c r="J41" s="13" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="K41" s="13" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="L41" s="15" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:12" ht="112.5" customHeight="1">
@@ -2444,7 +2464,7 @@
       <x:c r="F42" s="6"/>
       <x:c r="G42" s="6"/>
       <x:c r="H42" s="34" t="s">
-        <x:v>22</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I42" s="7"/>
       <x:c r="J42" s="6" t="s">
@@ -2455,7 +2475,7 @@
     </x:row>
     <x:row r="43" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A43" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B43" s="9"/>
       <x:c r="C43" s="10"/>
@@ -2466,14 +2486,14 @@
       <x:c r="H43" s="35"/>
       <x:c r="I43" s="5"/>
       <x:c r="J43" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="K43" s="8"/>
       <x:c r="L43" s="23"/>
     </x:row>
     <x:row r="44" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A44" s="18" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B44" s="19"/>
       <x:c r="C44" s="19"/>
@@ -2484,7 +2504,7 @@
       <x:c r="H44" s="36"/>
       <x:c r="I44" s="20"/>
       <x:c r="J44" s="21" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="K44" s="21"/>
       <x:c r="L44" s="24"/>

</xml_diff>

<commit_message>
2021-01-24 01:49 일정표 수정
</commit_message>
<xml_diff>
--- a/Communication/일정표(매일수정).xlsx
+++ b/Communication/일정표(매일수정).xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.5454"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="7710"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="28545" windowHeight="11880"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="30">
-  <x:si>
-    <x:t>9주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CSS 폼 디자인, UI 설계 및 시각적 기능 구현</x:t>
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="34">
+  <x:si>
+    <x:t>Boiler-Plate 안에 MongoDB 연동기능 추가예정</x:t>
   </x:si>
   <x:si>
     <x:t>환경구축 세팅
@@ -28,49 +25,53 @@
 MongoDB알아보기</x:t>
   </x:si>
   <x:si>
+    <x:t xml:space="preserve">지난 주말 환경셋팅을 다못하는 바람에 시간이 약간 새었음 </x:t>
+  </x:si>
+  <x:si>
+    <x:t>9주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>계획</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>날짜</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> </x:t>
+  </x:si>
+  <x:si>
+    <x:t>3주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8주차</x:t>
+  </x:si>
+  <x:si>
     <x:t>o</x:t>
   </x:si>
   <x:si>
-    <x:t>날짜</x:t>
-  </x:si>
-  <x:si>
-    <x:t>계획</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">지난 주말 환경셋팅을 다못하는 바람에 시간이 약간 새었음 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>문제점, 해결법</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">깃허브 생성 
-기능요구사항 토론
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">환경구축 세팅
-및 협의 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>오늘의 결과</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이번주 결과</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타 메모</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주간계획</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">부기능, 추가 희망기능 등등 추가하는 주 .() </x:t>
+    <x:t>4주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MongoDB 연동
+mongoose install
+express install
+body-Parser install
+postman다운</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Start : 
@@ -86,43 +87,61 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Boiler-Plate 제작</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8주차</x:t>
-  </x:si>
-  <x:si>
     <x:t>아무래도 밤늦게 진행하다 보니 졸리기도 하고 효율이 좋지 않은것 같다. 
 일찍하는게 좋지않나 싶다</x:t>
   </x:si>
   <x:si>
-    <x:t>3주차</x:t>
+    <x:t>문제점, 해결법</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">마감 - 발표 </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">참 한거 없네 </x:t>
   </x:si>
   <x:si>
-    <x:t>5주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">마감 - 발표 </x:t>
+    <x:t>CSS 폼 디자인, UI 설계 및 시각적 기능 구현</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">깃허브 생성 
+기능요구사항 토론
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타 메모</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이번주 결과</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오늘의 결과</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주간계획</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">부기능, 추가 희망기능 등등 추가하는 주 .() </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Boiler-Plate 제작</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">환경구축 세팅
+및 협의 </x:t>
   </x:si>
   <x:si>
     <x:t>환경구축 세팅 완료하기
 대략적 계획설립</x:t>
   </x:si>
   <x:si>
-    <x:t>2주차</x:t>
-  </x:si>
-  <x:si>
     <x:t>필수기능구현 및
 클라우드 기반 서버 구동</x:t>
   </x:si>
   <x:si>
-    <x:t>4주차</x:t>
+    <x:t>npm install mongoose --save
+npm install express --save
+npm install body-parser --save
+https://getpostman.com</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -312,12 +331,6 @@
       </x:patternFill>
     </x:fill>
     <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="ffffe766"/>
-        <x:bgColor indexed="64"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
       <x:patternFill patternType="lightUp">
         <x:fgColor rgb="ff000000"/>
         <x:bgColor rgb="ffcdf2e4"/>
@@ -341,6 +354,12 @@
         <x:bgColor indexed="64"/>
       </x:patternFill>
     </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="ffffe766"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
+    </x:fill>
   </x:fills>
   <x:borders count="11">
     <x:border>
@@ -548,7 +567,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="39">
+  <x:cellXfs count="47">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -735,13 +754,240 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
-    <x:xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="center" wrapText="1"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="164" fontId="7" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="164" fontId="7" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="general" vertical="center" wrapText="1"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center" wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center" wrapText="1"/>
+    </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="center" wrapText="1"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -752,136 +998,13 @@
     </x:xf>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <x:xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center" wrapText="1"/>
-    </x:xf>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="164" fontId="7" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="164" fontId="7" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <x:xf numFmtId="0" fontId="8" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="general" vertical="center" wrapText="1"/>
-    </x:xf>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+        <x:xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
@@ -1640,8 +1763,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="A1:M44"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D8" activeCellId="0" sqref="D8:D8"/>
+    <x:sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="L12" activeCellId="0" sqref="L12:L14"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
@@ -1658,7 +1781,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:12" s="3" customFormat="1" ht="114" customHeight="1">
       <x:c r="A1" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B1" s="13">
         <x:v>44200</x:v>
@@ -1683,91 +1806,91 @@
       </x:c>
       <x:c r="I1" s="14"/>
       <x:c r="J1" s="13" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="K1" s="13" t="s">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="L1" s="15" t="s">
-        <x:v>14</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:13" s="4" customFormat="1" ht="114" customHeight="1">
       <x:c r="A2" s="16" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B2" s="27"/>
-      <x:c r="C2" s="27"/>
-      <x:c r="D2" s="27"/>
-      <x:c r="E2" s="31" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F2" s="32" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G2" s="37" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="H2" s="32" t="s">
-        <x:v>11</x:v>
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="22"/>
+      <x:c r="C2" s="22"/>
+      <x:c r="D2" s="22"/>
+      <x:c r="E2" s="26" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="F2" s="27" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="G2" s="32" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H2" s="27" t="s">
+        <x:v>30</x:v>
       </x:c>
       <x:c r="I2" s="7"/>
       <x:c r="J2" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="K2" s="32" t="s">
-        <x:v>26</x:v>
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="K2" s="27" t="s">
+        <x:v>31</x:v>
       </x:c>
       <x:c r="L2" s="38" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="M2" s="25"/>
+      <x:c r="M2" s="44"/>
     </x:row>
     <x:row r="3" spans="1:13" s="3" customFormat="1" ht="114" customHeight="1">
       <x:c r="A3" s="17" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B3" s="28"/>
-      <x:c r="C3" s="29"/>
-      <x:c r="D3" s="29"/>
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B3" s="23"/>
+      <x:c r="C3" s="24"/>
+      <x:c r="D3" s="24"/>
       <x:c r="E3" s="9" t="s">
-        <x:v>3</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F3" s="9" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G3" s="9"/>
       <x:c r="H3" s="9"/>
       <x:c r="I3" s="5"/>
       <x:c r="J3" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K3" s="8"/>
-      <x:c r="L3" s="23"/>
-      <x:c r="M3" s="26"/>
+      <x:c r="L3" s="39"/>
+      <x:c r="M3" s="45"/>
     </x:row>
     <x:row r="4" spans="1:12" s="4" customFormat="1" ht="114" customHeight="1">
       <x:c r="A4" s="18" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B4" s="30"/>
-      <x:c r="C4" s="30"/>
-      <x:c r="D4" s="30"/>
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B4" s="25"/>
+      <x:c r="C4" s="25"/>
+      <x:c r="D4" s="25"/>
       <x:c r="E4" s="19"/>
       <x:c r="F4" s="19"/>
       <x:c r="G4" s="19"/>
       <x:c r="H4" s="19"/>
       <x:c r="I4" s="20"/>
       <x:c r="J4" s="21" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K4" s="21"/>
-      <x:c r="L4" s="24"/>
+      <x:c r="L4" s="40"/>
     </x:row>
     <x:row r="5" ht="23.25" customHeight="1"/>
-    <x:row r="6" spans="1:12" ht="91.5" customHeight="1">
+    <x:row r="6" spans="1:12" ht="116.25" customHeight="1">
       <x:c r="A6" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B6" s="13">
         <x:v>44207</x:v>
@@ -1790,49 +1913,59 @@
       <x:c r="H6" s="13">
         <x:v>44213</x:v>
       </x:c>
-      <x:c r="I6" s="14"/>
+      <x:c r="I6" s="34"/>
       <x:c r="J6" s="13" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="K6" s="13" t="s">
-        <x:v>27</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="L6" s="15" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:12" ht="91.5" customHeight="1">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:12" ht="116.25" customHeight="1">
       <x:c r="A7" s="16" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B7" s="6" t="s">
-        <x:v>18</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C7" s="6" t="s">
-        <x:v>18</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D7" s="6" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="E7" s="6"/>
-      <x:c r="F7" s="6"/>
-      <x:c r="G7" s="6"/>
-      <x:c r="H7" s="6"/>
-      <x:c r="I7" s="7"/>
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E7" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F7" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="G7" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="H7" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="I7" s="35"/>
       <x:c r="J7" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="K7" s="32" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="L7" s="22"/>
-    </x:row>
-    <x:row r="8" spans="1:12" ht="91.5" customHeight="1">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="K7" s="27" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="L7" s="38" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:12" ht="116.25" customHeight="1">
       <x:c r="A8" s="17" t="s">
-        <x:v>12</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B8" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="C8" s="10"/>
       <x:c r="D8" s="10"/>
@@ -1840,36 +1973,36 @@
       <x:c r="F8" s="9"/>
       <x:c r="G8" s="9"/>
       <x:c r="H8" s="9"/>
-      <x:c r="I8" s="5"/>
+      <x:c r="I8" s="36"/>
       <x:c r="J8" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K8" s="8"/>
-      <x:c r="L8" s="23"/>
-    </x:row>
-    <x:row r="9" spans="1:12" ht="91.5" customHeight="1">
+      <x:c r="L8" s="41"/>
+    </x:row>
+    <x:row r="9" spans="1:12" ht="116.25" customHeight="1">
       <x:c r="A9" s="18" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B9" s="19" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C9" s="19"/>
-      <x:c r="D9" s="19"/>
-      <x:c r="E9" s="19"/>
-      <x:c r="F9" s="19"/>
-      <x:c r="G9" s="19"/>
-      <x:c r="H9" s="19"/>
-      <x:c r="I9" s="20"/>
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B9" s="33" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C9" s="33"/>
+      <x:c r="D9" s="33"/>
+      <x:c r="E9" s="33"/>
+      <x:c r="F9" s="33"/>
+      <x:c r="G9" s="33"/>
+      <x:c r="H9" s="33"/>
+      <x:c r="I9" s="37"/>
       <x:c r="J9" s="21" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K9" s="21"/>
-      <x:c r="L9" s="24"/>
+      <x:c r="L9" s="42"/>
     </x:row>
     <x:row r="11" spans="1:12" ht="80.25" customHeight="1">
       <x:c r="A11" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="13">
         <x:v>44214</x:v>
@@ -1894,56 +2027,72 @@
       </x:c>
       <x:c r="I11" s="14"/>
       <x:c r="J11" s="13" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="K11" s="13" t="s">
-        <x:v>21</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="L11" s="15" t="s">
-        <x:v>14</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:12" ht="80.25" customHeight="1">
       <x:c r="A12" s="16" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B12" s="6"/>
-      <x:c r="C12" s="6"/>
-      <x:c r="D12" s="6"/>
-      <x:c r="E12" s="6"/>
-      <x:c r="F12" s="6"/>
-      <x:c r="G12" s="6"/>
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B12" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C12" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D12" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E12" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F12" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="G12" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
       <x:c r="H12" s="6"/>
       <x:c r="I12" s="7"/>
       <x:c r="J12" s="6" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="K12" s="6" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="L12" s="22"/>
-    </x:row>
-    <x:row r="13" spans="1:12" ht="80.25" customHeight="1">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="L12" s="43" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:12" ht="124.5" customHeight="1">
       <x:c r="A13" s="17" t="s">
-        <x:v>12</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B13" s="9"/>
       <x:c r="C13" s="10"/>
       <x:c r="D13" s="10"/>
       <x:c r="E13" s="11"/>
       <x:c r="F13" s="9"/>
-      <x:c r="G13" s="9"/>
+      <x:c r="G13" s="46" t="s">
+        <x:v>16</x:v>
+      </x:c>
       <x:c r="H13" s="9"/>
       <x:c r="I13" s="5"/>
       <x:c r="J13" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K13" s="8"/>
-      <x:c r="L13" s="23"/>
+      <x:c r="L13" s="39"/>
     </x:row>
     <x:row r="14" spans="1:12" ht="80.25" customHeight="1">
       <x:c r="A14" s="18" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B14" s="19"/>
       <x:c r="C14" s="19"/>
@@ -1954,14 +2103,14 @@
       <x:c r="H14" s="19"/>
       <x:c r="I14" s="20"/>
       <x:c r="J14" s="21" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K14" s="21"/>
-      <x:c r="L14" s="24"/>
+      <x:c r="L14" s="40"/>
     </x:row>
     <x:row r="16" spans="1:12" ht="81" customHeight="1">
       <x:c r="A16" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B16" s="13">
         <x:v>44221</x:v>
@@ -1986,18 +2135,18 @@
       </x:c>
       <x:c r="I16" s="14"/>
       <x:c r="J16" s="13" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K16" s="13" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="K16" s="13" t="s">
-        <x:v>29</x:v>
-      </x:c>
       <x:c r="L16" s="15" t="s">
-        <x:v>14</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:12" ht="81" customHeight="1">
       <x:c r="A17" s="16" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B17" s="6"/>
       <x:c r="C17" s="6"/>
@@ -2008,16 +2157,16 @@
       <x:c r="H17" s="6"/>
       <x:c r="I17" s="7"/>
       <x:c r="J17" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="K17" s="32" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="L17" s="22"/>
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="K17" s="27" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="L17" s="43"/>
     </x:row>
     <x:row r="18" spans="1:12" ht="81" customHeight="1">
       <x:c r="A18" s="17" t="s">
-        <x:v>12</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B18" s="9"/>
       <x:c r="C18" s="10"/>
@@ -2028,14 +2177,14 @@
       <x:c r="H18" s="9"/>
       <x:c r="I18" s="5"/>
       <x:c r="J18" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K18" s="8"/>
-      <x:c r="L18" s="23"/>
+      <x:c r="L18" s="39"/>
     </x:row>
     <x:row r="19" spans="1:12" ht="81" customHeight="1">
       <x:c r="A19" s="18" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B19" s="19"/>
       <x:c r="C19" s="19"/>
@@ -2046,14 +2195,14 @@
       <x:c r="H19" s="19"/>
       <x:c r="I19" s="20"/>
       <x:c r="J19" s="21" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K19" s="21"/>
-      <x:c r="L19" s="24"/>
+      <x:c r="L19" s="40"/>
     </x:row>
     <x:row r="21" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A21" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B21" s="13">
         <x:v>44228</x:v>
@@ -2078,18 +2227,18 @@
       </x:c>
       <x:c r="I21" s="14"/>
       <x:c r="J21" s="13" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="K21" s="13" t="s">
-        <x:v>23</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="L21" s="15" t="s">
-        <x:v>14</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A22" s="16" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B22" s="6"/>
       <x:c r="C22" s="6"/>
@@ -2100,16 +2249,16 @@
       <x:c r="H22" s="6"/>
       <x:c r="I22" s="7"/>
       <x:c r="J22" s="6" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="K22" s="6" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="L22" s="22"/>
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="L22" s="43"/>
     </x:row>
     <x:row r="23" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A23" s="17" t="s">
-        <x:v>12</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B23" s="9"/>
       <x:c r="C23" s="10"/>
@@ -2120,14 +2269,14 @@
       <x:c r="H23" s="9"/>
       <x:c r="I23" s="5"/>
       <x:c r="J23" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K23" s="8"/>
-      <x:c r="L23" s="23"/>
+      <x:c r="L23" s="39"/>
     </x:row>
     <x:row r="24" spans="1:12" ht="106.5" customHeight="1">
       <x:c r="A24" s="18" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B24" s="19"/>
       <x:c r="C24" s="19"/>
@@ -2138,14 +2287,14 @@
       <x:c r="H24" s="19"/>
       <x:c r="I24" s="20"/>
       <x:c r="J24" s="21" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K24" s="21"/>
-      <x:c r="L24" s="24"/>
+      <x:c r="L24" s="40"/>
     </x:row>
     <x:row r="26" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A26" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B26" s="13">
         <x:v>44235</x:v>
@@ -2170,18 +2319,18 @@
       </x:c>
       <x:c r="I26" s="14"/>
       <x:c r="J26" s="13" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="K26" s="13" t="s">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="L26" s="15" t="s">
-        <x:v>14</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A27" s="16" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B27" s="6"/>
       <x:c r="C27" s="6"/>
@@ -2192,16 +2341,16 @@
       <x:c r="H27" s="6"/>
       <x:c r="I27" s="7"/>
       <x:c r="J27" s="6" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="K27" s="6" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="L27" s="22"/>
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="L27" s="43"/>
     </x:row>
     <x:row r="28" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A28" s="17" t="s">
-        <x:v>12</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B28" s="9"/>
       <x:c r="C28" s="10"/>
@@ -2212,14 +2361,14 @@
       <x:c r="H28" s="9"/>
       <x:c r="I28" s="5"/>
       <x:c r="J28" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K28" s="8"/>
-      <x:c r="L28" s="23"/>
+      <x:c r="L28" s="39"/>
     </x:row>
     <x:row r="29" spans="1:12" ht="97.5" customHeight="1">
       <x:c r="A29" s="18" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B29" s="19"/>
       <x:c r="C29" s="19"/>
@@ -2230,14 +2379,14 @@
       <x:c r="H29" s="19"/>
       <x:c r="I29" s="20"/>
       <x:c r="J29" s="21" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K29" s="21"/>
-      <x:c r="L29" s="24"/>
+      <x:c r="L29" s="40"/>
     </x:row>
     <x:row r="31" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A31" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B31" s="13">
         <x:v>44242</x:v>
@@ -2262,18 +2411,18 @@
       </x:c>
       <x:c r="I31" s="14"/>
       <x:c r="J31" s="13" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="K31" s="13" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="L31" s="15" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="L31" s="15" t="s">
-        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A32" s="16" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B32" s="6"/>
       <x:c r="C32" s="6"/>
@@ -2284,16 +2433,16 @@
       <x:c r="H32" s="6"/>
       <x:c r="I32" s="7"/>
       <x:c r="J32" s="6" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="K32" s="6" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="L32" s="22"/>
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L32" s="43"/>
     </x:row>
     <x:row r="33" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A33" s="17" t="s">
-        <x:v>12</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B33" s="9"/>
       <x:c r="C33" s="10"/>
@@ -2304,14 +2453,14 @@
       <x:c r="H33" s="9"/>
       <x:c r="I33" s="5"/>
       <x:c r="J33" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K33" s="8"/>
-      <x:c r="L33" s="23"/>
+      <x:c r="L33" s="39"/>
     </x:row>
     <x:row r="34" spans="1:12" ht="108.75" customHeight="1">
       <x:c r="A34" s="18" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B34" s="19"/>
       <x:c r="C34" s="19"/>
@@ -2322,14 +2471,14 @@
       <x:c r="H34" s="19"/>
       <x:c r="I34" s="20"/>
       <x:c r="J34" s="21" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K34" s="21"/>
-      <x:c r="L34" s="24"/>
+      <x:c r="L34" s="40"/>
     </x:row>
     <x:row r="36" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A36" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B36" s="13">
         <x:v>44249</x:v>
@@ -2354,18 +2503,18 @@
       </x:c>
       <x:c r="I36" s="14"/>
       <x:c r="J36" s="13" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="K36" s="13" t="s">
-        <x:v>19</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="L36" s="15" t="s">
-        <x:v>14</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A37" s="16" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B37" s="6"/>
       <x:c r="C37" s="6"/>
@@ -2376,14 +2525,14 @@
       <x:c r="H37" s="6"/>
       <x:c r="I37" s="7"/>
       <x:c r="J37" s="6" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="K37" s="6"/>
-      <x:c r="L37" s="22"/>
+      <x:c r="L37" s="43"/>
     </x:row>
     <x:row r="38" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A38" s="17" t="s">
-        <x:v>12</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B38" s="9"/>
       <x:c r="C38" s="10"/>
@@ -2394,14 +2543,14 @@
       <x:c r="H38" s="9"/>
       <x:c r="I38" s="5"/>
       <x:c r="J38" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K38" s="8"/>
-      <x:c r="L38" s="23"/>
+      <x:c r="L38" s="39"/>
     </x:row>
     <x:row r="39" spans="1:12" ht="109.5" customHeight="1">
       <x:c r="A39" s="18" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B39" s="19"/>
       <x:c r="C39" s="19"/>
@@ -2412,14 +2561,14 @@
       <x:c r="H39" s="19"/>
       <x:c r="I39" s="20"/>
       <x:c r="J39" s="21" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K39" s="21"/>
-      <x:c r="L39" s="24"/>
+      <x:c r="L39" s="40"/>
     </x:row>
     <x:row r="41" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A41" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B41" s="13">
         <x:v>44256</x:v>
@@ -2439,23 +2588,23 @@
       <x:c r="G41" s="13">
         <x:v>44261</x:v>
       </x:c>
-      <x:c r="H41" s="33">
+      <x:c r="H41" s="28">
         <x:v>44262</x:v>
       </x:c>
       <x:c r="I41" s="14"/>
       <x:c r="J41" s="13" t="s">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="K41" s="13" t="s">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="L41" s="15" t="s">
-        <x:v>14</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A42" s="16" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B42" s="6"/>
       <x:c r="C42" s="6"/>
@@ -2463,19 +2612,19 @@
       <x:c r="E42" s="6"/>
       <x:c r="F42" s="6"/>
       <x:c r="G42" s="6"/>
-      <x:c r="H42" s="34" t="s">
-        <x:v>25</x:v>
+      <x:c r="H42" s="29" t="s">
+        <x:v>20</x:v>
       </x:c>
       <x:c r="I42" s="7"/>
       <x:c r="J42" s="6" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="K42" s="6"/>
-      <x:c r="L42" s="22"/>
+      <x:c r="L42" s="43"/>
     </x:row>
     <x:row r="43" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A43" s="17" t="s">
-        <x:v>12</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B43" s="9"/>
       <x:c r="C43" s="10"/>
@@ -2483,17 +2632,17 @@
       <x:c r="E43" s="11"/>
       <x:c r="F43" s="9"/>
       <x:c r="G43" s="9"/>
-      <x:c r="H43" s="35"/>
+      <x:c r="H43" s="30"/>
       <x:c r="I43" s="5"/>
       <x:c r="J43" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K43" s="8"/>
-      <x:c r="L43" s="23"/>
+      <x:c r="L43" s="39"/>
     </x:row>
     <x:row r="44" spans="1:12" ht="112.5" customHeight="1">
       <x:c r="A44" s="18" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B44" s="19"/>
       <x:c r="C44" s="19"/>
@@ -2501,13 +2650,13 @@
       <x:c r="E44" s="19"/>
       <x:c r="F44" s="19"/>
       <x:c r="G44" s="19"/>
-      <x:c r="H44" s="36"/>
+      <x:c r="H44" s="31"/>
       <x:c r="I44" s="20"/>
       <x:c r="J44" s="21" t="s">
-        <x:v>8</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K44" s="21"/>
-      <x:c r="L44" s="24"/>
+      <x:c r="L44" s="40"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="10">

</xml_diff>